<commit_message>
BOM had 0402 resistors, which should have been 0603. now fixed.
</commit_message>
<xml_diff>
--- a/microstim_BOM.xlsx
+++ b/microstim_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="137">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">1k</t>
   </si>
   <si>
-    <t xml:space="preserve"> RR0816P-102-D </t>
+    <t xml:space="preserve">RR0816P-102-D </t>
   </si>
   <si>
     <t xml:space="preserve">RR08P1.0KDCT-ND </t>
@@ -160,6 +160,9 @@
     <t xml:space="preserve">RR05P100DCT-ND </t>
   </si>
   <si>
+    <t xml:space="preserve">RR08P100DCT-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">R11,R14</t>
   </si>
   <si>
@@ -169,6 +172,9 @@
     <t xml:space="preserve">RR05P180DCT-ND </t>
   </si>
   <si>
+    <t xml:space="preserve">P180DBCT-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">R17,R18</t>
   </si>
   <si>
@@ -181,6 +187,9 @@
     <t xml:space="preserve">RR05P4.02KDCT-ND </t>
   </si>
   <si>
+    <t xml:space="preserve">P4.02KDBCT-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">U7</t>
   </si>
   <si>
@@ -418,10 +427,7 @@
     <t xml:space="preserve">B5-080BK</t>
   </si>
   <si>
-    <t xml:space="preserve">Main board PCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panel PCB</t>
+    <t xml:space="preserve">Combined PCB</t>
   </si>
   <si>
     <t xml:space="preserve">Total cost:</t>
@@ -559,10 +565,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -573,8 +579,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,6 +853,7 @@
         <f aca="false">H9*D9</f>
         <v>0.44</v>
       </c>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -875,13 +884,16 @@
         <f aca="false">H10*D10</f>
         <v>0.2</v>
       </c>
+      <c r="J10" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
@@ -893,10 +905,10 @@
         <v>180</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0.1</v>
@@ -905,13 +917,16 @@
         <f aca="false">H11*D11</f>
         <v>0.2</v>
       </c>
+      <c r="J11" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -920,13 +935,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>0.1</v>
@@ -935,28 +950,31 @@
         <f aca="false">H12*D12</f>
         <v>0.2</v>
       </c>
+      <c r="J12" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>4.32</v>
@@ -971,7 +989,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -980,13 +998,13 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>0.1</v>
@@ -995,13 +1013,14 @@
         <f aca="false">H14*D14</f>
         <v>0.7</v>
       </c>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
@@ -1010,13 +1029,13 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0.18</v>
@@ -1031,22 +1050,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>7.84</v>
@@ -1061,22 +1080,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>11.21</v>
@@ -1091,7 +1110,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>25</v>
@@ -1100,13 +1119,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0.48</v>
@@ -1121,7 +1140,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>25</v>
@@ -1130,13 +1149,13 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>0.44</v>
@@ -1151,22 +1170,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>4.44</v>
@@ -1181,7 +1200,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>25</v>
@@ -1190,13 +1209,13 @@
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>0.41</v>
@@ -1211,22 +1230,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>2.7</v>
@@ -1241,7 +1260,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>39</v>
@@ -1250,13 +1269,13 @@
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>0.8</v>
@@ -1271,7 +1290,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>39</v>
@@ -1283,10 +1302,10 @@
         <v>250</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>0.13</v>
@@ -1301,7 +1320,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
@@ -1310,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>2.73</v>
@@ -1331,7 +1350,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>25</v>
@@ -1340,13 +1359,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>2.81</v>
@@ -1361,22 +1380,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>2.43</v>
@@ -1386,7 +1405,7 @@
         <v>4.86</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1394,22 +1413,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>1.76</v>
@@ -1424,22 +1443,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>1.02</v>
@@ -1451,37 +1470,31 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="5" t="n">
+      <c r="D30" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E31" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H31" s="0" t="n">
+      <c r="E30" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H30" s="0" t="n">
         <v>2.67</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>18.71</v>
@@ -1493,27 +1506,29 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>6.298</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <f aca="false">H33*D33</f>
+        <v>62.98</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="D34" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H36" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I36" s="0" t="n">
         <f aca="false">SUM(I2:I34)</f>
-        <v>124.608</v>
+        <v>187.588</v>
       </c>
     </row>
   </sheetData>
@@ -1527,29 +1542,32 @@
     <hyperlink ref="G8" r:id="rId7" display="296-43866-1-ND"/>
     <hyperlink ref="G9" r:id="rId8" display="RR08P1.0KDCT-ND "/>
     <hyperlink ref="G10" r:id="rId9" display="RR05P100DCT-ND "/>
-    <hyperlink ref="G11" r:id="rId10" display="RR05P180DCT-ND "/>
-    <hyperlink ref="G12" r:id="rId11" display="RR05P4.02KDCT-ND "/>
-    <hyperlink ref="G13" r:id="rId12" display="296-47779-1-ND"/>
-    <hyperlink ref="G14" r:id="rId13" display="1276-1019-1-ND "/>
-    <hyperlink ref="G15" r:id="rId14" display="P20292CT-ND "/>
-    <hyperlink ref="G16" r:id="rId15" display="AD7321BRUZ-REEL7CT-ND "/>
-    <hyperlink ref="G17" r:id="rId16" display="445-2465-ND "/>
-    <hyperlink ref="G18" r:id="rId17" display="MC78L05ACDXCT-ND "/>
-    <hyperlink ref="G19" r:id="rId18" display="MC78L12ABDGOS-ND "/>
-    <hyperlink ref="G20" r:id="rId19" display="296-48142-1-ND "/>
-    <hyperlink ref="G21" r:id="rId20" display="MC79L12ACDR2GOSCT-ND "/>
-    <hyperlink ref="G22" r:id="rId21" display="MCP4922-E/SL-ND "/>
-    <hyperlink ref="G23" r:id="rId22" display="P3.0KBECT-ND "/>
-    <hyperlink ref="G24" r:id="rId23" display="P249BLCT-ND "/>
-    <hyperlink ref="G25" r:id="rId24" display="AD8276ARZ-ND "/>
-    <hyperlink ref="G26" r:id="rId25" display="296-30238-1-ND "/>
-    <hyperlink ref="G27" r:id="rId26" display="DG509BEY-T1-E3CT-ND "/>
-    <hyperlink ref="J27" r:id="rId27" display="DG409DY-T1-E3CT-ND "/>
-    <hyperlink ref="G28" r:id="rId28" display="AD1582ARTZREEL7CT-ND "/>
-    <hyperlink ref="G29" r:id="rId29" display="A123829-ND "/>
-    <hyperlink ref="F31" r:id="rId30" display="SSQ-124-03-T-S"/>
-    <hyperlink ref="G31" r:id="rId31" display="SAM1206-24-ND "/>
-    <hyperlink ref="G32" r:id="rId32" display="B5-080BK"/>
+    <hyperlink ref="J10" r:id="rId10" display="RR08P100DCT-ND "/>
+    <hyperlink ref="G11" r:id="rId11" display="RR05P180DCT-ND "/>
+    <hyperlink ref="J11" r:id="rId12" display="P180DBCT-ND "/>
+    <hyperlink ref="G12" r:id="rId13" display="RR05P4.02KDCT-ND "/>
+    <hyperlink ref="J12" r:id="rId14" display="P4.02KDBCT-ND "/>
+    <hyperlink ref="G13" r:id="rId15" display="296-47779-1-ND"/>
+    <hyperlink ref="G14" r:id="rId16" display="1276-1019-1-ND "/>
+    <hyperlink ref="G15" r:id="rId17" display="P20292CT-ND "/>
+    <hyperlink ref="G16" r:id="rId18" display="AD7321BRUZ-REEL7CT-ND "/>
+    <hyperlink ref="G17" r:id="rId19" display="445-2465-ND "/>
+    <hyperlink ref="G18" r:id="rId20" display="MC78L05ACDXCT-ND "/>
+    <hyperlink ref="G19" r:id="rId21" display="MC78L12ABDGOS-ND "/>
+    <hyperlink ref="G20" r:id="rId22" display="296-48142-1-ND "/>
+    <hyperlink ref="G21" r:id="rId23" display="MC79L12ACDR2GOSCT-ND "/>
+    <hyperlink ref="G22" r:id="rId24" display="MCP4922-E/SL-ND "/>
+    <hyperlink ref="G23" r:id="rId25" display="P3.0KBECT-ND "/>
+    <hyperlink ref="G24" r:id="rId26" display="P249BLCT-ND "/>
+    <hyperlink ref="G25" r:id="rId27" display="AD8276ARZ-ND "/>
+    <hyperlink ref="G26" r:id="rId28" display="296-30238-1-ND "/>
+    <hyperlink ref="G27" r:id="rId29" display="DG509BEY-T1-E3CT-ND "/>
+    <hyperlink ref="J27" r:id="rId30" display="DG409DY-T1-E3CT-ND "/>
+    <hyperlink ref="G28" r:id="rId31" display="AD1582ARTZREEL7CT-ND "/>
+    <hyperlink ref="G29" r:id="rId32" display="A123829-ND "/>
+    <hyperlink ref="F30" r:id="rId33" display="SSQ-124-03-T-S"/>
+    <hyperlink ref="G30" r:id="rId34" display="SAM1206-24-ND "/>
+    <hyperlink ref="G32" r:id="rId35" display="B5-080BK"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated readme, fixed BOM cost column for boards
</commit_message>
<xml_diff>
--- a/microstim_BOM.xlsx
+++ b/microstim_BOM.xlsx
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Total cost</t>
   </si>
   <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
@@ -157,9 +160,6 @@
     <t xml:space="preserve">RR0510P-101-D </t>
   </si>
   <si>
-    <t xml:space="preserve">RR05P100DCT-ND </t>
-  </si>
-  <si>
     <t xml:space="preserve">RR08P100DCT-ND </t>
   </si>
   <si>
@@ -169,9 +169,6 @@
     <t xml:space="preserve">RR0510P-181-D </t>
   </si>
   <si>
-    <t xml:space="preserve">RR05P180DCT-ND </t>
-  </si>
-  <si>
     <t xml:space="preserve">P180DBCT-ND </t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t xml:space="preserve">RR0510P-4021-D </t>
   </si>
   <si>
-    <t xml:space="preserve">RR05P4.02KDCT-ND </t>
-  </si>
-  <si>
     <t xml:space="preserve">P4.02KDBCT-ND </t>
   </si>
   <si>
@@ -379,7 +373,26 @@
     <t xml:space="preserve">DG509BEY-T1-E3CT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">DG409DY-T1-E3CT-ND </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Alternate part: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DG409DY-T1-E3CT-ND </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">U6</t>
@@ -424,10 +437,35 @@
     <t xml:space="preserve">Enclosure</t>
   </si>
   <si>
-    <t xml:space="preserve">B5-080BK</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Newark:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> B5-080BK</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Combined PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeedstudio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At quantity 10, total cost is 62.98</t>
   </si>
   <si>
     <t xml:space="preserve">Total cost:</t>
@@ -440,7 +478,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -474,6 +512,13 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -519,7 +564,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -540,11 +585,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -567,8 +616,8 @@
   </sheetPr>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -581,7 +630,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.26"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="39.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -613,28 +662,31 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>26.25</v>
@@ -649,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>731375003</v>
@@ -658,13 +710,13 @@
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>731375003</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1.48</v>
@@ -679,22 +731,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>885012206070</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0.1</v>
@@ -709,22 +761,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0.038</v>
@@ -739,22 +791,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>4.53</v>
@@ -769,22 +821,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0.4</v>
@@ -799,22 +851,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>1.6</v>
@@ -829,22 +881,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>0.11</v>
@@ -860,10 +912,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>2</v>
@@ -872,10 +924,10 @@
         <v>100</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="3" t="s">
         <v>45</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>0.1</v>
@@ -884,9 +936,6 @@
         <f aca="false">H10*D10</f>
         <v>0.2</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -896,7 +945,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>2</v>
@@ -907,7 +956,7 @@
       <c r="F11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="H11" s="0" t="n">
@@ -917,31 +966,28 @@
         <f aca="false">H11*D11</f>
         <v>0.2</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>0.1</v>
@@ -950,31 +996,28 @@
         <f aca="false">H12*D12</f>
         <v>0.2</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>4.32</v>
@@ -989,22 +1032,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>0.1</v>
@@ -1020,22 +1063,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0.18</v>
@@ -1050,22 +1093,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>7.84</v>
@@ -1080,22 +1123,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>11.21</v>
@@ -1110,22 +1153,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0.48</v>
@@ -1140,22 +1183,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>0.44</v>
@@ -1170,22 +1213,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>4.44</v>
@@ -1200,22 +1243,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>0.41</v>
@@ -1230,22 +1273,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>2.7</v>
@@ -1260,22 +1303,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>0.8</v>
@@ -1290,10 +1333,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>2</v>
@@ -1302,10 +1345,10 @@
         <v>250</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>0.13</v>
@@ -1320,22 +1363,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>2.73</v>
@@ -1350,22 +1393,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>2.81</v>
@@ -1380,22 +1423,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>2.43</v>
@@ -1404,8 +1447,8 @@
         <f aca="false">H27*D27</f>
         <v>4.86</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>119</v>
+      <c r="J27" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,22 +1456,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>1.76</v>
@@ -1443,22 +1486,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>1.02</v>
@@ -1470,17 +1513,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1"/>
-      <c r="D30" s="5" t="n">
+      <c r="D30" s="6" t="n">
         <v>4</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>2.67</v>
@@ -1488,13 +1531,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>134</v>
+      <c r="G32" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>18.71</v>
@@ -1506,17 +1549,23 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>6.298</v>
       </c>
       <c r="I33" s="0" t="n">
         <f aca="false">H33*D33</f>
-        <v>62.98</v>
+        <v>6.298</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,7 +1577,7 @@
       </c>
       <c r="I36" s="0" t="n">
         <f aca="false">SUM(I2:I34)</f>
-        <v>187.588</v>
+        <v>130.906</v>
       </c>
     </row>
   </sheetData>
@@ -1541,33 +1590,30 @@
     <hyperlink ref="G7" r:id="rId6" display="311-1376-1-ND "/>
     <hyperlink ref="G8" r:id="rId7" display="296-43866-1-ND"/>
     <hyperlink ref="G9" r:id="rId8" display="RR08P1.0KDCT-ND "/>
-    <hyperlink ref="G10" r:id="rId9" display="RR05P100DCT-ND "/>
-    <hyperlink ref="J10" r:id="rId10" display="RR08P100DCT-ND "/>
-    <hyperlink ref="G11" r:id="rId11" display="RR05P180DCT-ND "/>
-    <hyperlink ref="J11" r:id="rId12" display="P180DBCT-ND "/>
-    <hyperlink ref="G12" r:id="rId13" display="RR05P4.02KDCT-ND "/>
-    <hyperlink ref="J12" r:id="rId14" display="P4.02KDBCT-ND "/>
-    <hyperlink ref="G13" r:id="rId15" display="296-47779-1-ND"/>
-    <hyperlink ref="G14" r:id="rId16" display="1276-1019-1-ND "/>
-    <hyperlink ref="G15" r:id="rId17" display="P20292CT-ND "/>
-    <hyperlink ref="G16" r:id="rId18" display="AD7321BRUZ-REEL7CT-ND "/>
-    <hyperlink ref="G17" r:id="rId19" display="445-2465-ND "/>
-    <hyperlink ref="G18" r:id="rId20" display="MC78L05ACDXCT-ND "/>
-    <hyperlink ref="G19" r:id="rId21" display="MC78L12ABDGOS-ND "/>
-    <hyperlink ref="G20" r:id="rId22" display="296-48142-1-ND "/>
-    <hyperlink ref="G21" r:id="rId23" display="MC79L12ACDR2GOSCT-ND "/>
-    <hyperlink ref="G22" r:id="rId24" display="MCP4922-E/SL-ND "/>
-    <hyperlink ref="G23" r:id="rId25" display="P3.0KBECT-ND "/>
-    <hyperlink ref="G24" r:id="rId26" display="P249BLCT-ND "/>
-    <hyperlink ref="G25" r:id="rId27" display="AD8276ARZ-ND "/>
-    <hyperlink ref="G26" r:id="rId28" display="296-30238-1-ND "/>
-    <hyperlink ref="G27" r:id="rId29" display="DG509BEY-T1-E3CT-ND "/>
-    <hyperlink ref="J27" r:id="rId30" display="DG409DY-T1-E3CT-ND "/>
-    <hyperlink ref="G28" r:id="rId31" display="AD1582ARTZREEL7CT-ND "/>
-    <hyperlink ref="G29" r:id="rId32" display="A123829-ND "/>
-    <hyperlink ref="F30" r:id="rId33" display="SSQ-124-03-T-S"/>
-    <hyperlink ref="G30" r:id="rId34" display="SAM1206-24-ND "/>
-    <hyperlink ref="G32" r:id="rId35" display="B5-080BK"/>
+    <hyperlink ref="G10" r:id="rId9" display="RR08P100DCT-ND "/>
+    <hyperlink ref="G11" r:id="rId10" display="P180DBCT-ND "/>
+    <hyperlink ref="G12" r:id="rId11" display="P4.02KDBCT-ND "/>
+    <hyperlink ref="G13" r:id="rId12" display="296-47779-1-ND"/>
+    <hyperlink ref="G14" r:id="rId13" display="1276-1019-1-ND "/>
+    <hyperlink ref="G15" r:id="rId14" display="P20292CT-ND "/>
+    <hyperlink ref="G16" r:id="rId15" display="AD7321BRUZ-REEL7CT-ND "/>
+    <hyperlink ref="G17" r:id="rId16" display="445-2465-ND "/>
+    <hyperlink ref="G18" r:id="rId17" display="MC78L05ACDXCT-ND "/>
+    <hyperlink ref="G19" r:id="rId18" display="MC78L12ABDGOS-ND "/>
+    <hyperlink ref="G20" r:id="rId19" display="296-48142-1-ND "/>
+    <hyperlink ref="G21" r:id="rId20" display="MC79L12ACDR2GOSCT-ND "/>
+    <hyperlink ref="G22" r:id="rId21" display="MCP4922-E/SL-ND "/>
+    <hyperlink ref="G23" r:id="rId22" display="P3.0KBECT-ND "/>
+    <hyperlink ref="G24" r:id="rId23" display="P249BLCT-ND "/>
+    <hyperlink ref="G25" r:id="rId24" display="AD8276ARZ-ND "/>
+    <hyperlink ref="G26" r:id="rId25" display="296-30238-1-ND "/>
+    <hyperlink ref="G27" r:id="rId26" display="DG509BEY-T1-E3CT-ND "/>
+    <hyperlink ref="J27" r:id="rId27" display="DG409DY-T1-E3CT-ND "/>
+    <hyperlink ref="G28" r:id="rId28" display="AD1582ARTZREEL7CT-ND "/>
+    <hyperlink ref="G29" r:id="rId29" display="A123829-ND "/>
+    <hyperlink ref="F30" r:id="rId30" display="SSQ-124-03-T-S"/>
+    <hyperlink ref="G30" r:id="rId31" display="SAM1206-24-ND "/>
+    <hyperlink ref="G32" r:id="rId32" display="B5-080BK"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
increased board size to 129x79.5 from 124.5x79.5, changed enclosure to something on digikey rather than newark. also added trigger capability to teensy code
</commit_message>
<xml_diff>
--- a/microstim_BOM.xlsx
+++ b/microstim_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -433,7 +433,13 @@
     <t xml:space="preserve">Enclosure</t>
   </si>
   <si>
-    <t xml:space="preserve">Newark: B5-080BK</t>
+    <t xml:space="preserve">BOX ALUM CLR/SLV 3.5"L X 5.77"W </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXN-23359-SVP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">377-2550-ND</t>
   </si>
   <si>
     <t xml:space="preserve">Combined PCB</t>
@@ -538,7 +544,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -575,10 +581,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -599,7 +601,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1530,26 +1532,32 @@
       <c r="D31" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="E31" s="0" t="s">
         <v>137</v>
       </c>
+      <c r="F31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>139</v>
+      </c>
       <c r="H31" s="0" t="n">
-        <v>18.71</v>
+        <v>24.5</v>
       </c>
       <c r="I31" s="0" t="n">
         <f aca="false">H31*D31</f>
-        <v>18.71</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>6.298</v>
@@ -1559,13 +1567,13 @@
         <v>6.298</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I34" s="0" t="n">
         <f aca="false">SUM(I2:I32)</f>
-        <v>188.116</v>
+        <v>193.906</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1611,8 @@
     <hyperlink ref="G29" r:id="rId31" display="SAM1206-24-ND "/>
     <hyperlink ref="F30" r:id="rId32" display="PREC024SAAN-RC"/>
     <hyperlink ref="G30" r:id="rId33" display="S1012EC-24-ND "/>
-    <hyperlink ref="G31" r:id="rId34" display="Newark: B5-080BK"/>
+    <hyperlink ref="F31" r:id="rId34" display="EXN-23359-SVP"/>
+    <hyperlink ref="G31" r:id="rId35" display="377-2550-ND"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
boatload of updates via jons suggestions. de-isolated grounds via large resistors+capacitors (to prevent static buildup on animal or issues with large discharges). increased resistor values in voltage output non-inverting amplifier.
</commit_message>
<xml_diff>
--- a/microstim_BOM.xlsx
+++ b/microstim_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="152">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -313,7 +313,7 @@
     <t xml:space="preserve">WM5514-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R8,R14,R7</t>
+    <t xml:space="preserve">R14,R7</t>
   </si>
   <si>
     <t xml:space="preserve">1k</t>
@@ -325,13 +325,40 @@
     <t xml:space="preserve">RR08P1.0KDCT-ND </t>
   </si>
   <si>
+    <t xml:space="preserve">R1,R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
     <t xml:space="preserve">R3,R10</t>
   </si>
   <si>
-    <t xml:space="preserve">RR0816P-4990-D-68A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RR08P499DCT-ND </t>
+    <t xml:space="preserve">5k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21,R17,R19,R20,R22,R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_1210_3225Metric_Pad1.42x2.65mm_HandSolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_Small_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">541-2312-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C53,C54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_Disc_D12.5mm_W5.0mm_P10.00mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399-9520-1-ND </t>
   </si>
   <si>
     <t xml:space="preserve">R13,R6</t>
@@ -598,10 +625,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1252,328 +1279,372 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>21</v>
-      </c>
       <c r="B22" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="D22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <f aca="false">H22*D22</f>
-        <v>0.22</v>
-      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="D24" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="0" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <f aca="false">H23*D23</f>
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" s="0" t="s">
+      <c r="G24" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="H24" s="0" t="n">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="C25" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H24" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <f aca="false">H24*D24</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" s="0" t="s">
+      <c r="D25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="G25" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>2.73</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <f aca="false">H25*D25</f>
-        <v>5.46</v>
+      <c r="H25" s="4" t="n">
+        <v>0.78</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="G26" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="H26" s="0" t="n">
-        <v>2.81</v>
+        <v>0.11</v>
       </c>
       <c r="I26" s="0" t="n">
         <f aca="false">H26*D26</f>
-        <v>5.62</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="H27" s="0" t="n">
-        <v>2.43</v>
+        <v>0.1</v>
       </c>
       <c r="I27" s="0" t="n">
         <f aca="false">H27*D27</f>
-        <v>4.86</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>124</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>200</v>
+        <v>2</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>0.11</v>
+        <v>2.73</v>
       </c>
       <c r="I28" s="0" t="n">
         <f aca="false">H28*D28</f>
-        <v>0.44</v>
-      </c>
-      <c r="J28" s="7"/>
+        <v>5.46</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>131</v>
+        <v>30</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>2.67</v>
+        <v>2.81</v>
       </c>
       <c r="I29" s="0" t="n">
         <f aca="false">H29*D29</f>
-        <v>5.34</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D30" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="H30" s="0" t="n">
-        <v>0.46</v>
+        <v>2.43</v>
       </c>
       <c r="I30" s="0" t="n">
         <f aca="false">H30*D30</f>
-        <v>0.92</v>
+        <v>4.86</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>27</v>
+      </c>
       <c r="B31" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>139</v>
-      </c>
       <c r="H31" s="0" t="n">
-        <v>24.5</v>
+        <v>0.11</v>
       </c>
       <c r="I31" s="0" t="n">
         <f aca="false">H31*D31</f>
-        <v>24.5</v>
-      </c>
+        <v>0.44</v>
+      </c>
+      <c r="J31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="B32" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D32" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>141</v>
-      </c>
       <c r="H32" s="0" t="n">
-        <v>6.298</v>
+        <v>2.67</v>
       </c>
       <c r="I32" s="0" t="n">
         <f aca="false">H32*D32</f>
+        <v>5.34</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <f aca="false">H33*D33</f>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <f aca="false">H34*D34</f>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="H35" s="0" t="n">
         <v>6.298</v>
       </c>
-      <c r="J32" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I34" s="0" t="n">
-        <f aca="false">SUM(I2:I32)</f>
-        <v>193.906</v>
+      <c r="I35" s="0" t="n">
+        <f aca="false">H35*D35</f>
+        <v>6.298</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="0" t="n">
+        <f aca="false">SUM(I2:I35)</f>
+        <v>193.686</v>
       </c>
     </row>
   </sheetData>
@@ -1599,20 +1670,21 @@
     <hyperlink ref="G19" r:id="rId19" display="1568-1443-ND "/>
     <hyperlink ref="G20" r:id="rId20" display="WM5514-ND"/>
     <hyperlink ref="G21" r:id="rId21" display="RR08P1.0KDCT-ND "/>
-    <hyperlink ref="G22" r:id="rId22" display="RR08P499DCT-ND "/>
-    <hyperlink ref="G23" r:id="rId23" display="RR08P1.8KDCT-ND "/>
-    <hyperlink ref="G24" r:id="rId24" display="RR08P100DCT-ND "/>
-    <hyperlink ref="G25" r:id="rId25" display="AD8276ARZ-ND "/>
-    <hyperlink ref="G26" r:id="rId26" display="296-30238-1-ND "/>
-    <hyperlink ref="G27" r:id="rId27" display="DG509BEY-T1-E3CT-ND "/>
-    <hyperlink ref="J27" r:id="rId28" display="Alternate part: DG409DY-T1-E3CT-ND "/>
-    <hyperlink ref="G28" r:id="rId29" display="RR08P200DCT-ND "/>
-    <hyperlink ref="F29" r:id="rId30" display="SSQ-124-03-T-S"/>
-    <hyperlink ref="G29" r:id="rId31" display="SAM1206-24-ND "/>
-    <hyperlink ref="F30" r:id="rId32" display="PREC024SAAN-RC"/>
-    <hyperlink ref="G30" r:id="rId33" display="S1012EC-24-ND "/>
-    <hyperlink ref="F31" r:id="rId34" display="EXN-23359-SVP"/>
-    <hyperlink ref="G31" r:id="rId35" display="377-2550-ND"/>
+    <hyperlink ref="G24" r:id="rId22" display="541-2312-1-ND"/>
+    <hyperlink ref="G25" r:id="rId23" display="399-9520-1-ND "/>
+    <hyperlink ref="G26" r:id="rId24" display="RR08P1.8KDCT-ND "/>
+    <hyperlink ref="G27" r:id="rId25" display="RR08P100DCT-ND "/>
+    <hyperlink ref="G28" r:id="rId26" display="AD8276ARZ-ND "/>
+    <hyperlink ref="G29" r:id="rId27" display="296-30238-1-ND "/>
+    <hyperlink ref="G30" r:id="rId28" display="DG509BEY-T1-E3CT-ND "/>
+    <hyperlink ref="J30" r:id="rId29" display="Alternate part: DG409DY-T1-E3CT-ND "/>
+    <hyperlink ref="G31" r:id="rId30" display="RR08P200DCT-ND "/>
+    <hyperlink ref="F32" r:id="rId31" display="SSQ-124-03-T-S"/>
+    <hyperlink ref="G32" r:id="rId32" display="SAM1206-24-ND "/>
+    <hyperlink ref="F33" r:id="rId33" display="PREC024SAAN-RC"/>
+    <hyperlink ref="G33" r:id="rId34" display="S1012EC-24-ND "/>
+    <hyperlink ref="F34" r:id="rId35" display="EXN-23359-SVP"/>
+    <hyperlink ref="G34" r:id="rId36" display="377-2550-ND"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>